<commit_message>
[ADD]complete second point the login
</commit_message>
<xml_diff>
--- a/src/main/resources/inputData.xlsx
+++ b/src/main/resources/inputData.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="UsuariosRegistro" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="LoginData" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Nombre</t>
   </si>
@@ -35,6 +36,18 @@
   </si>
   <si>
     <t>juan@gmail.com</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>test1@gmail.com</t>
+  </si>
+  <si>
+    <t>invalido</t>
   </si>
 </sst>
 </file>
@@ -84,6 +97,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -331,4 +348,44 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="16.38"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1">
+        <v>123456.0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se creó una clase por cada pagina. Se colocaron los selectores como atributos de cada clase y se añadieron validaciones
</commit_message>
<xml_diff>
--- a/src/main/resources/inputData.xlsx
+++ b/src/main/resources/inputData.xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correousbcaliedu-my.sharepoint.com/personal/mdmorar_correo_usbcali_edu_co/Documents/Archivos Universidad/Ingeniería De Sistemas/Semestre 6/Calidad y Pruebas Software/Proyecto Final/Opencart-automatic/src/main/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="65" documentId="11_7BA5C62F2122C8D10D4A2E9F72BB96FB370B5C7B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A1AB8A5-26C6-4597-AB11-79747F2802F8}"/>
+  <bookViews>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="UsuariosRegistro" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="LoginData" sheetId="2" r:id="rId5"/>
+    <sheet name="UsuariosRegistro" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginData" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Nombre</t>
   </si>
@@ -29,41 +38,82 @@
     <t>Contraseña</t>
   </si>
   <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Perez</t>
-  </si>
-  <si>
-    <t>juan@gmail.com</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
     <t>Tipo</t>
   </si>
   <si>
-    <t>test1@gmail.com</t>
-  </si>
-  <si>
-    <t>invalido</t>
+    <t>Valido</t>
+  </si>
+  <si>
+    <t>Nombre1</t>
+  </si>
+  <si>
+    <t>Apellido2</t>
+  </si>
+  <si>
+    <t>Apellido1</t>
+  </si>
+  <si>
+    <t>Nombre2</t>
+  </si>
+  <si>
+    <t>Nombre3</t>
+  </si>
+  <si>
+    <t>Apellido3</t>
+  </si>
+  <si>
+    <t>valido</t>
+  </si>
+  <si>
+    <t>prueba12@correo.com.co</t>
+  </si>
+  <si>
+    <t>prueba22@correo.com.co</t>
+  </si>
+  <si>
+    <t>prueba33@correo.com.co</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -72,40 +122,51 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -295,23 +356,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="15.63"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -328,64 +394,134 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1">
-        <v>3.042134768E9</v>
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>34342424</v>
       </c>
       <c r="E2" s="1">
-        <v>123456.0</v>
+        <v>48375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>34342424</v>
+      </c>
+      <c r="E3" s="1">
+        <v>48375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>34342424</v>
+      </c>
+      <c r="E4" s="1">
+        <v>48375</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{220CB8E9-87D3-4905-8EC8-CF826E37FBB7}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{EF10D263-F316-4458-BCF5-8278072313C2}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{7CA8C914-FC7A-4722-AFD2-D1E85B71D47C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.38"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="1">
-        <v>123456.0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>48375</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>48375</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1">
+        <v>48375</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{02A8CB5C-8BF6-49FF-A7FA-4DEFC42CDE3A}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{7EEDA291-2756-4EDD-9952-05A572156C13}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{95A4F16E-10ED-4F15-AA01-828882942E26}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agregada la busqueda y la agregación al carrito
</commit_message>
<xml_diff>
--- a/src/main/resources/inputData.xlsx
+++ b/src/main/resources/inputData.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correousbcaliedu-my.sharepoint.com/personal/mdmorar_correo_usbcali_edu_co/Documents/Archivos Universidad/Ingeniería De Sistemas/Semestre 6/Calidad y Pruebas Software/Proyecto Final/Opencart-automatic/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="11_7BA5C62F2122C8D10D4A2E9F72BB96FB370B5C7B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A1AB8A5-26C6-4597-AB11-79747F2802F8}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="11_7BA5C62F2122C8D10D4A2E9F72BB96FB370B5C7B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA0E6902-7400-4080-B2A5-51411F5B9450}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UsuariosRegistro" sheetId="1" r:id="rId1"/>
     <sheet name="LoginData" sheetId="2" r:id="rId2"/>
+    <sheet name="Productos" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Nombre</t>
   </si>
@@ -75,6 +76,15 @@
   </si>
   <si>
     <t>prueba33@correo.com.co</t>
+  </si>
+  <si>
+    <t>Iphone</t>
+  </si>
+  <si>
+    <t>MacBook</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Tab</t>
   </si>
 </sst>
 </file>
@@ -368,7 +378,7 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -524,4 +534,39 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EF6C5E-F4AA-4FFA-9FC9-EC64664214AE}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
arreglado carrito page y test
</commit_message>
<xml_diff>
--- a/src/main/resources/inputData.xlsx
+++ b/src/main/resources/inputData.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correousbcaliedu-my.sharepoint.com/personal/mdmorar_correo_usbcali_edu_co/Documents/Archivos Universidad/Ingeniería De Sistemas/Semestre 6/Calidad y Pruebas Software/Proyecto Final/Opencart-automatic/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="11_7BA5C62F2122C8D10D4A2E9F72BB96FB370B5C7B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA0E6902-7400-4080-B2A5-51411F5B9450}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="11_7BA5C62F2122C8D10D4A2E9F72BB96FB370B5C7B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B0216C2-4882-41AF-AFF7-A531774D3C24}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UsuariosRegistro" sheetId="1" r:id="rId1"/>
     <sheet name="LoginData" sheetId="2" r:id="rId2"/>
     <sheet name="Productos" sheetId="3" r:id="rId3"/>
+    <sheet name="ProductosCarrito" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Nombre</t>
   </si>
@@ -171,10 +172,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -371,6 +368,53 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="0" row="0">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{679FC1DD-7BCD-482E-B3B5-376930CD582C}">
+  <we:reference id="wa200005502" version="1.0.0.11" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="WA200005502" version="1.0.0.11" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_GPT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_LIST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_HLIST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_CLASSIFY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_TRANSLATE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_EXTRACT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_TAG</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_CONVERT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_FORMAT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_SUMMARIZE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_TABLE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_FILL</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_SPLIT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_HSPLIT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_EDIT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_MATCH</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_VISION</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_WEB</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
@@ -540,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EF6C5E-F4AA-4FFA-9FC9-EC64664214AE}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -569,4 +613,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83596CFE-9586-4796-B5FB-E28432B5DD0F}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>